<commit_message>
All 10 lessons JetPack Fundamental JetPack.xlsx
</commit_message>
<xml_diff>
--- a/Android Kotlin Fundamentals/JetPack.xlsx
+++ b/Android Kotlin Fundamentals/JetPack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72761D29-2F71-4E6E-9EC4-8C5A29A79E7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDC4DD3-60E5-4A78-84FD-9E537CF32B57}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="185">
   <si>
     <t>Откуда</t>
   </si>
@@ -391,12 +391,6 @@
     <t>L 10: Desiging</t>
   </si>
   <si>
-    <t>andfun-kotlin-gdg-finder-u</t>
-  </si>
-  <si>
-    <t>andfun-kotlin-gdg-finder-u2</t>
-  </si>
-  <si>
     <t>GDGFinderFinal</t>
   </si>
   <si>
@@ -536,6 +530,51 @@
   </si>
   <si>
     <t>Мой исправленный коммент</t>
+  </si>
+  <si>
+    <t>Со всеми комментариями</t>
+  </si>
+  <si>
+    <t>Первая со всеми комментами</t>
+  </si>
+  <si>
+    <t>Glide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English </t>
+  </si>
+  <si>
+    <t>English Codelabs</t>
+  </si>
+  <si>
+    <t>не разбирал с фото</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Первый с выпол</t>
+  </si>
+  <si>
+    <t>раб Codelabs English</t>
+  </si>
+  <si>
+    <t>раб Udacity English mat 1,0,0</t>
+  </si>
+  <si>
+    <t>Последний mat 1,1,0</t>
+  </si>
+  <si>
+    <t>Неверный URL</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Preload Fonts</t>
+  </si>
+  <si>
+    <t>English Codelabs Final</t>
   </si>
 </sst>
 </file>
@@ -591,7 +630,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,6 +655,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -630,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -662,6 +707,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -943,11 +990,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X76"/>
+  <dimension ref="A1:AA74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -962,7 +1009,7 @@
     <col min="24" max="24" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="5" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -998,7 +1045,7 @@
         <v>40</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>64</v>
@@ -1013,25 +1060,34 @@
         <v>70</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="T1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="V1" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="26.25" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -1049,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1075,7 +1131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1096,7 +1152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
         <v>16</v>
@@ -1114,7 +1170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1155,7 +1211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1193,7 +1249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1231,7 +1287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>27</v>
       </c>
@@ -1269,7 +1325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1307,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -1345,7 +1401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1380,7 +1436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>37</v>
       </c>
@@ -1412,7 +1468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>36</v>
       </c>
@@ -2125,10 +2181,10 @@
         <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
@@ -2143,7 +2199,7 @@
         <v>5</v>
       </c>
       <c r="I34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J34" t="s">
         <v>5</v>
@@ -2181,10 +2237,10 @@
         <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E35" t="s">
         <v>49</v>
@@ -2199,7 +2255,7 @@
         <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J35" t="s">
         <v>5</v>
@@ -2237,10 +2293,10 @@
         <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E36" t="s">
         <v>5</v>
@@ -2255,7 +2311,7 @@
         <v>5</v>
       </c>
       <c r="I36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J36" t="s">
         <v>5</v>
@@ -2293,10 +2349,10 @@
         <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E37" t="s">
         <v>49</v>
@@ -2311,7 +2367,7 @@
         <v>49</v>
       </c>
       <c r="I37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J37" t="s">
         <v>5</v>
@@ -2352,7 +2408,7 @@
         <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E39" t="s">
         <v>5</v>
@@ -2370,7 +2426,7 @@
         <v>6</v>
       </c>
       <c r="J39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K39" t="s">
         <v>6</v>
@@ -2417,7 +2473,7 @@
         <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
@@ -2435,7 +2491,7 @@
         <v>6</v>
       </c>
       <c r="J40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K40" t="s">
         <v>6</v>
@@ -2482,7 +2538,7 @@
         <v>104</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E41" t="s">
         <v>5</v>
@@ -2500,7 +2556,7 @@
         <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K41" t="s">
         <v>6</v>
@@ -2547,7 +2603,7 @@
         <v>105</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E42" t="s">
         <v>5</v>
@@ -2565,7 +2621,7 @@
         <v>6</v>
       </c>
       <c r="J42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K42" t="s">
         <v>6</v>
@@ -2615,10 +2671,10 @@
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E44" t="s">
         <v>49</v>
@@ -2674,13 +2730,13 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E45" t="s">
         <v>49</v>
@@ -2739,7 +2795,7 @@
         <v>102</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E46" t="s">
         <v>49</v>
@@ -2798,13 +2854,13 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C47" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
@@ -2812,89 +2868,89 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B49" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" t="s">
+        <v>5</v>
+      </c>
+      <c r="I49" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49" t="s">
+        <v>5</v>
+      </c>
+      <c r="K49" t="s">
+        <v>49</v>
+      </c>
+      <c r="L49" t="s">
+        <v>49</v>
+      </c>
+      <c r="M49" t="s">
+        <v>49</v>
+      </c>
+      <c r="N49" t="s">
+        <v>5</v>
+      </c>
+      <c r="O49" t="s">
+        <v>5</v>
+      </c>
+      <c r="P49" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>5</v>
+      </c>
+      <c r="R49" t="s">
+        <v>5</v>
+      </c>
+      <c r="S49" t="s">
+        <v>5</v>
+      </c>
+      <c r="T49" t="s">
+        <v>6</v>
+      </c>
+      <c r="U49" t="s">
+        <v>152</v>
+      </c>
+      <c r="V49" t="s">
+        <v>6</v>
+      </c>
+      <c r="W49" t="s">
+        <v>6</v>
+      </c>
+      <c r="X49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C48" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" t="s">
-        <v>150</v>
-      </c>
-      <c r="E49" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" t="s">
-        <v>5</v>
-      </c>
-      <c r="G49" t="s">
-        <v>5</v>
-      </c>
-      <c r="H49" t="s">
-        <v>5</v>
-      </c>
-      <c r="I49" t="s">
-        <v>5</v>
-      </c>
-      <c r="J49" t="s">
-        <v>5</v>
-      </c>
-      <c r="K49" t="s">
-        <v>49</v>
-      </c>
-      <c r="L49" t="s">
-        <v>49</v>
-      </c>
-      <c r="M49" t="s">
-        <v>49</v>
-      </c>
-      <c r="N49" t="s">
-        <v>5</v>
-      </c>
-      <c r="O49" t="s">
-        <v>5</v>
-      </c>
-      <c r="P49" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>5</v>
-      </c>
-      <c r="R49" t="s">
-        <v>5</v>
-      </c>
-      <c r="S49" t="s">
-        <v>5</v>
-      </c>
-      <c r="T49" t="s">
-        <v>6</v>
-      </c>
-      <c r="U49" t="s">
+      <c r="C50" t="s">
         <v>154</v>
       </c>
-      <c r="V49" t="s">
-        <v>6</v>
-      </c>
-      <c r="W49" t="s">
-        <v>6</v>
-      </c>
-      <c r="X49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>106</v>
       </c>
@@ -2902,7 +2958,7 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E52" t="s">
         <v>5</v>
@@ -2965,12 +3021,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E53" t="s">
         <v>5</v>
@@ -3033,12 +3089,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B54" s="11" t="s">
         <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E54" t="s">
         <v>5</v>
@@ -3101,16 +3157,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C55" t="s">
+        <v>163</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="E55" t="s">
         <v>6</v>
       </c>
@@ -3172,16 +3228,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
         <v>109</v>
       </c>
       <c r="C56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="E56" t="s">
         <v>6</v>
       </c>
@@ -3243,93 +3299,431 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+      <c r="C59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B60" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B62" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>170</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" t="s">
+        <v>6</v>
+      </c>
+      <c r="I62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" t="s">
+        <v>6</v>
+      </c>
+      <c r="K62" t="s">
+        <v>6</v>
+      </c>
+      <c r="L62" t="s">
+        <v>6</v>
+      </c>
+      <c r="M62" t="s">
+        <v>6</v>
+      </c>
+      <c r="N62" t="s">
+        <v>5</v>
+      </c>
+      <c r="O62" t="s">
+        <v>6</v>
+      </c>
+      <c r="P62" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>6</v>
+      </c>
+      <c r="R62" t="s">
+        <v>5</v>
+      </c>
+      <c r="S62" t="s">
+        <v>5</v>
+      </c>
+      <c r="T62" t="s">
+        <v>5</v>
+      </c>
+      <c r="U62" t="s">
+        <v>6</v>
+      </c>
+      <c r="V62" t="s">
+        <v>5</v>
+      </c>
+      <c r="W62" t="s">
+        <v>5</v>
+      </c>
+      <c r="X62" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="15" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3" t="s">
+      <c r="C64" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B65" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" t="s">
+        <v>180</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" t="s">
+        <v>6</v>
+      </c>
+      <c r="J65" t="s">
+        <v>6</v>
+      </c>
+      <c r="K65" t="s">
+        <v>6</v>
+      </c>
+      <c r="L65" t="s">
+        <v>6</v>
+      </c>
+      <c r="M65" t="s">
+        <v>6</v>
+      </c>
+      <c r="P65" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>8</v>
+      </c>
+      <c r="R65" t="s">
+        <v>5</v>
+      </c>
+      <c r="S65" t="s">
+        <v>5</v>
+      </c>
+      <c r="T65" t="s">
+        <v>6</v>
+      </c>
+      <c r="U65" t="s">
+        <v>6</v>
+      </c>
+      <c r="V65" t="s">
+        <v>6</v>
+      </c>
+      <c r="W65" t="s">
+        <v>6</v>
+      </c>
+      <c r="X65" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" t="s">
+        <v>177</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" t="s">
+        <v>6</v>
+      </c>
+      <c r="I66" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66" t="s">
+        <v>6</v>
+      </c>
+      <c r="K66" t="s">
+        <v>6</v>
+      </c>
+      <c r="L66" t="s">
+        <v>6</v>
+      </c>
+      <c r="M66" t="s">
+        <v>6</v>
+      </c>
+      <c r="P66" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>8</v>
+      </c>
+      <c r="R66" t="s">
+        <v>5</v>
+      </c>
+      <c r="S66" t="s">
+        <v>5</v>
+      </c>
+      <c r="T66" t="s">
+        <v>6</v>
+      </c>
+      <c r="U66" t="s">
+        <v>6</v>
+      </c>
+      <c r="V66" t="s">
+        <v>6</v>
+      </c>
+      <c r="W66" t="s">
+        <v>6</v>
+      </c>
+      <c r="X66" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" t="s">
+        <v>178</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>175</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" t="s">
+        <v>6</v>
+      </c>
+      <c r="I68" t="s">
+        <v>6</v>
+      </c>
+      <c r="K68" t="s">
+        <v>6</v>
+      </c>
+      <c r="L68" t="s">
+        <v>6</v>
+      </c>
+      <c r="M68" t="s">
+        <v>6</v>
+      </c>
+      <c r="N68" t="s">
+        <v>6</v>
+      </c>
+      <c r="O68" t="s">
+        <v>5</v>
+      </c>
+      <c r="P68" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>5</v>
+      </c>
+      <c r="R68" t="s">
+        <v>5</v>
+      </c>
+      <c r="S68" t="s">
+        <v>5</v>
+      </c>
+      <c r="T68" t="s">
+        <v>5</v>
+      </c>
+      <c r="U68" t="s">
+        <v>176</v>
+      </c>
+      <c r="V68" t="s">
+        <v>12</v>
+      </c>
+      <c r="W68" t="s">
+        <v>6</v>
+      </c>
+      <c r="X68" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3" t="s">
+      <c r="C70" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B71" s="11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3" t="s">
+      <c r="C71" t="s">
+        <v>181</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" t="s">
+        <v>6</v>
+      </c>
+      <c r="J71" t="s">
+        <v>6</v>
+      </c>
+      <c r="K71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L71" t="s">
+        <v>6</v>
+      </c>
+      <c r="M71" t="s">
+        <v>6</v>
+      </c>
+      <c r="O71" t="s">
+        <v>6</v>
+      </c>
+      <c r="P71" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>6</v>
+      </c>
+      <c r="R71" t="s">
+        <v>12</v>
+      </c>
+      <c r="T71" t="s">
+        <v>12</v>
+      </c>
+      <c r="U71" t="s">
+        <v>6</v>
+      </c>
+      <c r="V71" t="s">
+        <v>6</v>
+      </c>
+      <c r="W71" t="s">
+        <v>12</v>
+      </c>
+      <c r="X71" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3" t="s">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lesson 12 Coroutines 1
</commit_message>
<xml_diff>
--- a/Android Kotlin Fundamentals/JetPack.xlsx
+++ b/Android Kotlin Fundamentals/JetPack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDC4DD3-60E5-4A78-84FD-9E537CF32B57}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F10135-E485-4776-A717-3E9A34AA524E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="186">
   <si>
     <t>Откуда</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t>English Codelabs Final</t>
+  </si>
+  <si>
+    <t>https://tutorialwing.com/java-kotlin-android-tutorial-examples/</t>
   </si>
 </sst>
 </file>
@@ -990,11 +993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA74"/>
+  <dimension ref="A1:AA80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3724,6 +3727,16 @@
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Android Basics with Compose 2023 start
</commit_message>
<xml_diff>
--- a/Android Kotlin Fundamentals/JetPack.xlsx
+++ b/Android Kotlin Fundamentals/JetPack.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F10135-E485-4776-A717-3E9A34AA524E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A698CCA5-2ACE-4749-8EE8-36FF85EDF565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14640" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="187">
   <si>
     <t>Откуда</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>https://tutorialwing.com/java-kotlin-android-tutorial-examples/</t>
+  </si>
+  <si>
+    <t>https://developer.android.com/courses/kotlin-android-fundamentals/toc</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -710,7 +713,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -996,8 +998,8 @@
   <dimension ref="A1:AA80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1090,6 +1092,11 @@
         <v>183</v>
       </c>
     </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
     <row r="4" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
@@ -3418,7 +3425,7 @@
       <c r="A64" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C64" t="s">
@@ -3570,7 +3577,7 @@
       <c r="A68" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C68" t="s">

</xml_diff>